<commit_message>
Incorporated a few changes
</commit_message>
<xml_diff>
--- a/BMS-UKI/lib/xlFiles/UKI_QC_Results.xlsx
+++ b/BMS-UKI/lib/xlFiles/UKI_QC_Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ys19299\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ys19299\git\GeneralLearnings\BMS-UKI\lib\xlFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{343DFCB7-E930-45BB-83F8-DE3764235137}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
+  <xr:revisionPtr documentId="13_ncr:1_{745C949A-36E3-47BA-BC23-CD072CD4671A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="1" windowHeight="9804" windowWidth="21912" xWindow="7092" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1260"/>
+    <workbookView activeTab="5" firstSheet="1" windowHeight="13176" windowWidth="22128" xWindow="1020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="Login Config" r:id="rId1" sheetId="6" state="hidden"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="72">
   <si>
     <t>Dashboard</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>40.6%</t>
+  </si>
+  <si>
+    <t>56.2%</t>
   </si>
 </sst>
 </file>
@@ -692,7 +695,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -798,6 +801,9 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="20" fillId="3" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="20" fillId="3" fontId="5" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="21" fillId="3" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -839,7 +845,7 @@
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -859,60 +865,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <border>
@@ -1730,27 +1682,23 @@
   <sheetPr codeName="Sheet6">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:V19"/>
+  <dimension ref="B1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row ht="15" r="1" spans="2:21" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="15" r="1" spans="2:17" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L1" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="46"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-    </row>
-    <row ht="15" r="2" spans="2:21" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row ht="15" r="2" spans="2:17" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>30</v>
       </c>
@@ -1782,38 +1730,23 @@
         <v>62</v>
       </c>
       <c r="L2" s="41">
-        <v>43964</v>
-      </c>
-      <c r="M2" s="41">
-        <v>43965</v>
-      </c>
-      <c r="N2" s="41">
-        <v>43966</v>
-      </c>
-      <c r="O2" s="41">
-        <v>43967</v>
-      </c>
-      <c r="P2" s="41">
-        <v>43968</v>
-      </c>
-      <c r="Q2" s="35" t="s">
+        <v>43972</v>
+      </c>
+      <c r="M2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="35" t="s">
+      <c r="N2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="35" t="s">
+      <c r="O2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="35" t="s">
+      <c r="P2" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="2"/>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3">
       <c r="B3" t="s">
         <v>31</v>
       </c>
@@ -1844,25 +1777,11 @@
       <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" t="s">
+      <c r="L3" t="s">
         <v>70</v>
       </c>
-      <c r="P3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
+    </row>
+    <row r="4">
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -1893,21 +1812,11 @@
       <c r="K4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
+      <c r="L4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="B5" t="s">
         <v>31</v>
       </c>
@@ -1938,60 +1847,15 @@
       <c r="K5" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="42"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D19" s="1"/>
+      <c r="L5"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="L1:P1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B3:K5">
-    <cfRule dxfId="9" priority="3" type="expression">
-      <formula>NOT(ISBLANK(B4))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:U4">
-    <cfRule dxfId="8" priority="1" type="expression">
-      <formula>NOT(ISBLANK(L4))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L5:U5">
-    <cfRule dxfId="7" priority="2" type="expression">
-      <formula>NOT(ISBLANK(#REF!))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -2023,13 +1887,13 @@
       <c r="G1" s="2"/>
       <c r="H1" s="36"/>
       <c r="I1" s="36"/>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="47"/>
     </row>
     <row customFormat="1" ht="15" r="2" s="2" spans="2:19" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
@@ -3552,16 +3416,16 @@
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="54" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="13" t="s">
@@ -3580,10 +3444,10 @@
       <c r="L10" s="27"/>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C11" s="49"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="54"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="55"/>
       <c r="G11" s="13" t="s">
         <v>12</v>
       </c>
@@ -3600,10 +3464,10 @@
       <c r="L11" s="27"/>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C12" s="49"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="54"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="55"/>
       <c r="G12" s="13" t="s">
         <v>13</v>
       </c>
@@ -3620,10 +3484,10 @@
       <c r="L12" s="27"/>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="49"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="54"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="55"/>
       <c r="G13" s="13" t="s">
         <v>14</v>
       </c>
@@ -3638,10 +3502,10 @@
       <c r="L13" s="27"/>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C14" s="49"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="54"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="55"/>
       <c r="G14" s="13" t="s">
         <v>15</v>
       </c>
@@ -3658,10 +3522,10 @@
       <c r="L14" s="27"/>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C15" s="49"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="54"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="55"/>
       <c r="G15" s="13" t="s">
         <v>16</v>
       </c>
@@ -3678,10 +3542,10 @@
       <c r="L15" s="27"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C16" s="49"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="13" t="s">
         <v>17</v>
       </c>
@@ -3698,10 +3562,10 @@
       <c r="L16" s="27"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C17" s="50"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="47" t="s">
+      <c r="C17" s="51"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="48" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="15" t="s">
@@ -3720,10 +3584,10 @@
       <c r="L17" s="30"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C18" s="50"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="54"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="55"/>
       <c r="G18" s="15" t="s">
         <v>12</v>
       </c>
@@ -3740,10 +3604,10 @@
       <c r="L18" s="30"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C19" s="50"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="55"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="56"/>
       <c r="G19" s="15" t="s">
         <v>19</v>
       </c>
@@ -3762,8 +3626,8 @@
       <c r="L19" s="30"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C20" s="50"/>
-      <c r="D20" s="55"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="56"/>
       <c r="E20" s="17" t="s">
         <v>41</v>
       </c>
@@ -3788,14 +3652,14 @@
       </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C21" s="50"/>
-      <c r="D21" s="47" t="s">
+      <c r="C21" s="51"/>
+      <c r="D21" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="47" t="s">
+      <c r="E21" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="47" t="s">
+      <c r="F21" s="48" t="s">
         <v>42</v>
       </c>
       <c r="G21" s="17" t="s">
@@ -3818,10 +3682,10 @@
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C22" s="50"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
       <c r="G22" s="17" t="s">
         <v>49</v>
       </c>
@@ -3838,10 +3702,10 @@
       <c r="L22" s="31"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C23" s="50"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
       <c r="G23" s="17" t="s">
         <v>50</v>
       </c>
@@ -3858,10 +3722,10 @@
       <c r="L23" s="31"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C24" s="50"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
       <c r="G24" s="17" t="s">
         <v>51</v>
       </c>
@@ -3882,12 +3746,12 @@
       </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C25" s="50"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="47" t="s">
+      <c r="C25" s="51"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="47" t="s">
+      <c r="F25" s="48" t="s">
         <v>52</v>
       </c>
       <c r="G25" s="17" t="s">
@@ -3906,10 +3770,10 @@
       <c r="L25" s="31"/>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C26" s="51"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
       <c r="G26" s="19" t="s">
         <v>51</v>
       </c>
@@ -3930,12 +3794,12 @@
       </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C27" s="51"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="47" t="s">
+      <c r="C27" s="52"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="47" t="s">
+      <c r="F27" s="48" t="s">
         <v>55</v>
       </c>
       <c r="G27" s="19" t="s">
@@ -3956,10 +3820,10 @@
       <c r="L27" s="33"/>
     </row>
     <row ht="15" r="28" spans="3:12" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="52"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
       <c r="G28" s="21" t="s">
         <v>53</v>
       </c>

</xml_diff>